<commit_message>
Final layout done and Gerbers generated
</commit_message>
<xml_diff>
--- a/v1.0/thingBot-LoRa_v1P0.xlsx
+++ b/v1.0/thingBot-LoRa_v1P0.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="71">
   <si>
     <t>BILL OF MATERIALS</t>
   </si>
@@ -231,9 +231,6 @@
   </si>
   <si>
     <t xml:space="preserve">thingBot-LoRa </t>
-  </si>
-  <si>
-    <t>purchased cost</t>
   </si>
 </sst>
 </file>
@@ -311,7 +308,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -371,22 +368,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -433,12 +419,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -741,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,10 +738,9 @@
     <col min="8" max="8" width="12.7109375" customWidth="1"/>
     <col min="9" max="9" width="43" customWidth="1"/>
     <col min="10" max="10" width="11.7109375" customWidth="1"/>
-    <col min="18" max="18" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:17" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="13" t="s">
         <v>70</v>
       </c>
@@ -782,7 +761,7 @@
       <c r="P1" s="14"/>
       <c r="Q1" s="15"/>
     </row>
-    <row r="2" spans="1:18" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:17" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
@@ -803,7 +782,7 @@
       <c r="P2" s="17"/>
       <c r="Q2" s="18"/>
     </row>
-    <row r="3" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -853,11 +832,8 @@
       <c r="Q3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="R3" s="19" t="s">
-        <v>71</v>
-      </c>
     </row>
-    <row r="4" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -907,11 +883,8 @@
       <c r="Q4" s="9">
         <v>1.19</v>
       </c>
-      <c r="R4" s="20">
-        <v>0.6</v>
-      </c>
     </row>
-    <row r="5" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>2</v>
       </c>
@@ -961,11 +934,8 @@
       <c r="Q5" s="9">
         <v>1.1200000000000001</v>
       </c>
-      <c r="R5" s="20">
-        <v>0.5</v>
-      </c>
     </row>
-    <row r="6" spans="1:18" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>3</v>
       </c>
@@ -1015,11 +985,8 @@
       <c r="Q6" s="9">
         <v>4.13</v>
       </c>
-      <c r="R6" s="20">
-        <v>1.2</v>
-      </c>
     </row>
-    <row r="7" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>4</v>
       </c>
@@ -1070,7 +1037,7 @@
         <v>5.18</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>5</v>
       </c>
@@ -1121,7 +1088,7 @@
         <v>38.64</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>6</v>
       </c>
@@ -1170,7 +1137,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>7</v>
       </c>
@@ -1219,7 +1186,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>8</v>
       </c>
@@ -1268,7 +1235,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>9</v>
       </c>
@@ -1317,7 +1284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>10</v>
       </c>
@@ -1364,7 +1331,7 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>11</v>
       </c>
@@ -1413,7 +1380,7 @@
         <v>2.66</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M16" s="12"/>
       <c r="N16" s="12" t="s">
         <v>69</v>

</xml_diff>